<commit_message>
Criação de Arquivos Base = Pronta
</commit_message>
<xml_diff>
--- a/Documentação/Backlog1.1.xlsx
+++ b/Documentação/Backlog1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno_t_santos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno_t_santos\Desktop\F1_novo\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
-  <si>
-    <t>lista de tarefas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
   <si>
     <t>identificar as configurações de desempenho do jogo - Atualização - requisito não funcional</t>
   </si>
@@ -218,6 +215,18 @@
   </si>
   <si>
     <t>Inicialização do Projeto</t>
+  </si>
+  <si>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>style.css</t>
+  </si>
+  <si>
+    <t>f1_main.js</t>
+  </si>
+  <si>
+    <t>f1_class.js</t>
   </si>
 </sst>
 </file>
@@ -267,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -290,11 +299,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -303,6 +321,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,90 +625,90 @@
   <sheetData>
     <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -693,7 +717,7 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -702,7 +726,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -711,7 +735,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -720,7 +744,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -729,7 +753,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -738,7 +762,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -747,7 +771,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -756,7 +780,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -765,7 +789,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -774,7 +798,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -783,7 +807,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -799,18 +823,18 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -826,7 +850,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -835,7 +859,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -850,10 +874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F27"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,260 +887,329 @@
     <col min="6" max="6" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A24:A27"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1141,157 +1234,157 @@
   <sheetData>
     <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1303,18 +1396,18 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1326,14 +1419,14 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>

</xml_diff>